<commit_message>
Update the Features section of the README and add screenshots.  Also store the excel source for the test cases and feature matrix
</commit_message>
<xml_diff>
--- a/documentation/matrix 1.xlsx
+++ b/documentation/matrix 1.xlsx
@@ -1074,6 +1074,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1086,13 +1090,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1409,18 +1409,18 @@
   <sheetData>
     <row r="2" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="8"/>
@@ -1456,7 +1456,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1478,7 +1478,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="20"/>
       <c r="B5" s="3" t="s">
         <v>212</v>
       </c>
@@ -1498,7 +1498,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="20"/>
       <c r="B6" s="3" t="s">
         <v>213</v>
       </c>
@@ -1518,7 +1518,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="20"/>
       <c r="B7" s="3" t="s">
         <v>214</v>
       </c>
@@ -1536,7 +1536,7 @@
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
+      <c r="A8" s="20"/>
       <c r="B8" s="3" t="s">
         <v>215</v>
       </c>
@@ -1556,7 +1556,7 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
+      <c r="A9" s="20"/>
       <c r="B9" s="3" t="s">
         <v>216</v>
       </c>
@@ -1574,7 +1574,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="A10" s="20"/>
       <c r="B10" s="3" t="s">
         <v>217</v>
       </c>
@@ -1596,7 +1596,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="3" t="s">
         <v>218</v>
       </c>
@@ -1614,7 +1614,7 @@
       <c r="L11" s="2"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="3" t="s">
         <v>219</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="3" t="s">
         <v>220</v>
       </c>
@@ -1650,8 +1650,8 @@
       <c r="L13" s="2"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="20"/>
+      <c r="B14" s="15" t="s">
         <v>221</v>
       </c>
       <c r="C14" s="3"/>
@@ -1681,8 +1681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="G63" sqref="G63"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,7 +2788,7 @@
       <c r="E55" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="F55" s="18" t="s">
+      <c r="F55" s="14" t="s">
         <v>203</v>
       </c>
       <c r="G55" s="11" t="s">

</xml_diff>